<commit_message>
Added enum and nullable enum support. Some refactoring Added reading of string-representation of enum
</commit_message>
<xml_diff>
--- a/ExcelDataReader.ReadToClass.Tests/Resources/Sample_OneSheet_Nullable.xlsx
+++ b/ExcelDataReader.ReadToClass.Tests/Resources/Sample_OneSheet_Nullable.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stuff\repos\ExcelDataReader.ReadToClass\ExcelDataReader.ReadToClass.Tests\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="My Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913" iterateCount="250" iterateDelta="1E-8"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Text Column</t>
   </si>
@@ -52,12 +57,15 @@
   </si>
   <si>
     <t>Hodor</t>
+  </si>
+  <si>
+    <t>Nullable Enums</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -106,6 +114,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -153,7 +164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,7 +199,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -411,7 +422,7 @@
     <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +435,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -440,8 +454,11 @@
         <f>IF(MOD(B2,3)=0,"",B2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -456,8 +473,11 @@
         <f t="shared" ref="D3:D8" si="0">IF(MOD(B3,3)=0,"",B3)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -472,8 +492,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -489,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -504,8 +527,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -520,8 +546,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -535,6 +564,9 @@
       <c r="D8">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>